<commit_message>
add info in excel files
</commit_message>
<xml_diff>
--- a/excel_files/clients.xlsx
+++ b/excel_files/clients.xlsx
@@ -1,33 +1,117 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jscy\Desktop\bootcamp_project\Schedule-System\excel_files\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="11760" windowWidth="20730" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
-    <sheet name="clients" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="clients" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="145621" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>Mimi</t>
+  </si>
+  <si>
+    <t>Nono</t>
+  </si>
+  <si>
+    <t>Lili</t>
+  </si>
+  <si>
+    <t>Zozo</t>
+  </si>
+  <si>
+    <t>Riri</t>
+  </si>
+  <si>
+    <t>Suzi</t>
+  </si>
+  <si>
+    <t>Nana</t>
+  </si>
+  <si>
+    <t>Fifi</t>
+  </si>
+  <si>
+    <t>Kimo</t>
+  </si>
+  <si>
+    <t>Simo</t>
+  </si>
+  <si>
+    <t>Rimi</t>
+  </si>
+  <si>
+    <t>10,20</t>
+  </si>
+  <si>
+    <t>30,50</t>
+  </si>
+  <si>
+    <t>20,20</t>
+  </si>
+  <si>
+    <t>10,10</t>
+  </si>
+  <si>
+    <t>70,10</t>
+  </si>
+  <si>
+    <t>10,80</t>
+  </si>
+  <si>
+    <t>50,50</t>
+  </si>
+  <si>
+    <t>100,20</t>
+  </si>
+  <si>
+    <t>70,20</t>
+  </si>
+  <si>
+    <t>60,50</t>
+  </si>
+  <si>
+    <t>200,50</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -43,15 +127,30 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -310,184 +409,160 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" max="2" min="2" width="15.5703125"/>
+    <col min="1" max="1" width="15.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>location</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Mimi</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>123456789</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>0,20</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Nono</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>33344</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>30,75</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>err</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>63859</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>99</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>djfdj</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>75412</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>8,9</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>aSdASHD</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>78258</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>6,6</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>suzi</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>84850</v>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>wiki</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>d444</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>TESTCLIENT</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>2,5</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>TESTCLIENT</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>86312</v>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>2,5</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>TESTCLIENT22</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>8229</v>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>22,5</t>
-        </is>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1">
+        <v>12345</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1">
+        <v>12346</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1">
+        <v>12347</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1">
+        <v>12348</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1">
+        <v>12349</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="1">
+        <v>32145</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="1">
+        <v>32146</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="1">
+        <v>32149</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="1">
+        <v>65478</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="1">
+        <v>65421</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="1">
+        <v>96325</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updating info in excel files
</commit_message>
<xml_diff>
--- a/excel_files/clients.xlsx
+++ b/excel_files/clients.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jscy\Desktop\bootcamp_project\Schedule-System\excel_files\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
@@ -33,73 +28,73 @@
     <t>Mimi</t>
   </si>
   <si>
+    <t>10,20</t>
+  </si>
+  <si>
     <t>Nono</t>
   </si>
   <si>
+    <t>30,50</t>
+  </si>
+  <si>
     <t>Lili</t>
   </si>
   <si>
+    <t>20,20</t>
+  </si>
+  <si>
     <t>Zozo</t>
   </si>
   <si>
+    <t>10,10</t>
+  </si>
+  <si>
     <t>Riri</t>
   </si>
   <si>
+    <t>70,10</t>
+  </si>
+  <si>
     <t>Suzi</t>
   </si>
   <si>
+    <t>10,80</t>
+  </si>
+  <si>
     <t>Nana</t>
   </si>
   <si>
+    <t>50,50</t>
+  </si>
+  <si>
     <t>Fifi</t>
   </si>
   <si>
+    <t>100,20</t>
+  </si>
+  <si>
     <t>Kimo</t>
   </si>
   <si>
+    <t>200,50</t>
+  </si>
+  <si>
     <t>Simo</t>
   </si>
   <si>
+    <t>70,20</t>
+  </si>
+  <si>
     <t>Rimi</t>
   </si>
   <si>
-    <t>10,20</t>
-  </si>
-  <si>
-    <t>30,50</t>
-  </si>
-  <si>
-    <t>20,20</t>
-  </si>
-  <si>
-    <t>10,10</t>
-  </si>
-  <si>
-    <t>70,10</t>
-  </si>
-  <si>
-    <t>10,80</t>
-  </si>
-  <si>
-    <t>50,50</t>
-  </si>
-  <si>
-    <t>100,20</t>
-  </si>
-  <si>
-    <t>70,20</t>
-  </si>
-  <si>
     <t>60,50</t>
-  </si>
-  <si>
-    <t>200,50</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -146,9 +141,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -197,7 +189,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -232,7 +224,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -409,7 +401,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -420,7 +412,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -449,100 +441,100 @@
         <v>12345</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1">
         <v>12346</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1">
         <v>12347</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B5" s="1">
         <v>12348</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B6" s="1">
         <v>12349</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B7" s="1">
         <v>32145</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B8" s="1">
         <v>32146</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B9" s="1">
         <v>32149</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="B10" s="1">
         <v>65478</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="B11" s="1">
         <v>65421</v>
@@ -553,13 +545,13 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B12" s="1">
         <v>96325</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating info in excel file
</commit_message>
<xml_diff>
--- a/excel_files/clients.xlsx
+++ b/excel_files/clients.xlsx
@@ -1,112 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="11760" windowWidth="20730" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="clients" sheetId="1" r:id="rId1"/>
+    <sheet name="clients" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>location</t>
-  </si>
-  <si>
-    <t>Mimi</t>
-  </si>
-  <si>
-    <t>10,20</t>
-  </si>
-  <si>
-    <t>Nono</t>
-  </si>
-  <si>
-    <t>30,50</t>
-  </si>
-  <si>
-    <t>Lili</t>
-  </si>
-  <si>
-    <t>20,20</t>
-  </si>
-  <si>
-    <t>Zozo</t>
-  </si>
-  <si>
-    <t>10,10</t>
-  </si>
-  <si>
-    <t>Riri</t>
-  </si>
-  <si>
-    <t>70,10</t>
-  </si>
-  <si>
-    <t>Suzi</t>
-  </si>
-  <si>
-    <t>10,80</t>
-  </si>
-  <si>
-    <t>Nana</t>
-  </si>
-  <si>
-    <t>50,50</t>
-  </si>
-  <si>
-    <t>Fifi</t>
-  </si>
-  <si>
-    <t>100,20</t>
-  </si>
-  <si>
-    <t>Kimo</t>
-  </si>
-  <si>
-    <t>200,50</t>
-  </si>
-  <si>
-    <t>Simo</t>
-  </si>
-  <si>
-    <t>70,20</t>
-  </si>
-  <si>
-    <t>Rimi</t>
-  </si>
-  <si>
-    <t>60,50</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -122,27 +43,21 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
 </styleSheet>
 </file>
 
@@ -408,153 +323,222 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" customWidth="1"/>
+    <col customWidth="1" max="1" min="1" width="15.42578125"/>
+    <col customWidth="1" max="2" min="2" width="15.5703125"/>
+    <col customWidth="1" max="3" min="3" width="14.140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1">
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>location</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Mimi</t>
+        </is>
+      </c>
+      <c r="B2" s="1" t="n">
         <v>12345</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="1">
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>10,20</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Nono</t>
+        </is>
+      </c>
+      <c r="B3" s="1" t="n">
         <v>12346</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="1">
+      <c r="C3" s="1" t="inlineStr">
+        <is>
+          <t>30,50</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>Lili</t>
+        </is>
+      </c>
+      <c r="B4" s="1" t="n">
         <v>12347</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="1">
+      <c r="C4" s="1" t="inlineStr">
+        <is>
+          <t>20,20</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>Zozo</t>
+        </is>
+      </c>
+      <c r="B5" s="1" t="n">
         <v>12348</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="1">
+      <c r="C5" s="1" t="inlineStr">
+        <is>
+          <t>10,10</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Riri</t>
+        </is>
+      </c>
+      <c r="B6" s="1" t="n">
         <v>12349</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="1">
+      <c r="C6" s="1" t="inlineStr">
+        <is>
+          <t>70,10</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Suzi</t>
+        </is>
+      </c>
+      <c r="B7" s="1" t="n">
         <v>32145</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="1">
+      <c r="C7" s="1" t="inlineStr">
+        <is>
+          <t>10,80</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>Nana</t>
+        </is>
+      </c>
+      <c r="B8" s="1" t="n">
         <v>32146</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="1">
+      <c r="C8" s="1" t="inlineStr">
+        <is>
+          <t>50,50</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>Fifi</t>
+        </is>
+      </c>
+      <c r="B9" s="1" t="n">
         <v>32149</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="1">
+      <c r="C9" s="1" t="inlineStr">
+        <is>
+          <t>100,20</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>Kimo</t>
+        </is>
+      </c>
+      <c r="B10" s="1" t="n">
         <v>65478</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="1">
+      <c r="C10" s="2" t="inlineStr">
+        <is>
+          <t>200,50</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>Simo</t>
+        </is>
+      </c>
+      <c r="B11" s="1" t="n">
         <v>65421</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" s="1">
+      <c r="C11" s="1" t="inlineStr">
+        <is>
+          <t>70,20</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>Rimi</t>
+        </is>
+      </c>
+      <c r="B12" s="1" t="n">
         <v>96325</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>24</v>
+      <c r="C12" s="1" t="inlineStr">
+        <is>
+          <t>60,50</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>82479</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>30,40</t>
+        </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>